<commit_message>
Fix create user from excel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\EduGate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24B7785-27FA-4357-BABA-11DCC283AF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65337F09-5777-4802-ACD5-88D66C01B50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="2685" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>FirstName</t>
   </si>
@@ -289,13 +289,19 @@
   </si>
   <si>
     <t>0943210987</t>
+  </si>
+  <si>
+    <t>Nam 1</t>
+  </si>
+  <si>
+    <t>nam@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +314,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -342,10 +356,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -366,8 +381,12 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -646,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,8 +1101,53 @@
       </c>
       <c r="O11" s="1"/>
     </row>
+    <row r="12" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="3">
+        <v>27729</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2">
+        <v>2</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1" xr:uid="{01B6E2CD-AC89-45EC-857F-9316D87C2B02}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{110F4B36-A89E-4B89-8928-C89AAD0497E1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>